<commit_message>
doing v2 and v3 and more qualities; adding min length and max length to fish release
</commit_message>
<xml_diff>
--- a/intermediateTables/鱼单价工具-moreQualities.xlsx
+++ b/intermediateTables/鱼单价工具-moreQualities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DocsHDD\FGame\中鱼\StatDemo\intermediateTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDE9B69C-A762-4CC3-9F6A-5E3B61676A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225BA388-D36C-4794-8888-46E123DC2F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1103,7 +1103,7 @@
             <v>1</v>
           </cell>
           <cell r="J2">
-            <v>1000</v>
+            <v>2200</v>
           </cell>
           <cell r="K2">
             <v>148</v>
@@ -1138,7 +1138,7 @@
             <v>1</v>
           </cell>
           <cell r="J3">
-            <v>1000</v>
+            <v>1800</v>
           </cell>
           <cell r="K3">
             <v>177</v>
@@ -1160,6 +1160,7 @@
           <cell r="E4">
             <v>1.7</v>
           </cell>
+          <cell r="F4"/>
           <cell r="G4">
             <v>340</v>
           </cell>
@@ -1192,6 +1193,7 @@
           <cell r="E5">
             <v>1.5</v>
           </cell>
+          <cell r="F5"/>
           <cell r="G5">
             <v>300</v>
           </cell>
@@ -1224,6 +1226,7 @@
           <cell r="E6">
             <v>2</v>
           </cell>
+          <cell r="F6"/>
           <cell r="G6">
             <v>400</v>
           </cell>
@@ -1256,6 +1259,7 @@
           <cell r="E7">
             <v>2.2999999999999998</v>
           </cell>
+          <cell r="F7"/>
           <cell r="G7">
             <v>460</v>
           </cell>
@@ -1288,6 +1292,7 @@
           <cell r="E8">
             <v>3</v>
           </cell>
+          <cell r="F8"/>
           <cell r="G8">
             <v>800</v>
           </cell>
@@ -1320,6 +1325,7 @@
           <cell r="E9">
             <v>3</v>
           </cell>
+          <cell r="F9"/>
           <cell r="G9">
             <v>800</v>
           </cell>
@@ -1352,6 +1358,7 @@
           <cell r="E10">
             <v>3.5</v>
           </cell>
+          <cell r="F10"/>
           <cell r="G10">
             <v>1000</v>
           </cell>
@@ -1384,6 +1391,7 @@
           <cell r="E11">
             <v>4</v>
           </cell>
+          <cell r="F11"/>
           <cell r="G11">
             <v>1600</v>
           </cell>
@@ -1416,6 +1424,7 @@
           <cell r="E12">
             <v>4.3</v>
           </cell>
+          <cell r="F12"/>
           <cell r="G12">
             <v>1800</v>
           </cell>
@@ -1437,7 +1446,7 @@
         </row>
         <row r="13">
           <cell r="B13" t="str">
-            <v>美鳊</v>
+            <v>灰西鲱</v>
           </cell>
           <cell r="C13" t="str">
             <v>保底</v>
@@ -1448,6 +1457,9 @@
           <cell r="E13">
             <v>1</v>
           </cell>
+          <cell r="F13" t="str">
+            <v>开放水域游动的保底鱼</v>
+          </cell>
           <cell r="G13">
             <v>200</v>
           </cell>
@@ -1458,7 +1470,7 @@
             <v>2</v>
           </cell>
           <cell r="J13">
-            <v>1000</v>
+            <v>2200</v>
           </cell>
           <cell r="K13">
             <v>148</v>
@@ -1469,19 +1481,20 @@
         </row>
         <row r="14">
           <cell r="B14" t="str">
-            <v>蓝鳃太阳鱼</v>
+            <v>美鳊</v>
           </cell>
           <cell r="C14" t="str">
             <v>保底</v>
           </cell>
           <cell r="D14">
-            <v>2</v>
+            <v>1</v>
           </cell>
           <cell r="E14">
-            <v>2</v>
-          </cell>
+            <v>1</v>
+          </cell>
+          <cell r="F14"/>
           <cell r="G14">
-            <v>400</v>
+            <v>200</v>
           </cell>
           <cell r="H14" t="str">
             <v>1、2</v>
@@ -1490,30 +1503,31 @@
             <v>2</v>
           </cell>
           <cell r="J14">
-            <v>1000</v>
+            <v>1800</v>
           </cell>
           <cell r="K14">
-            <v>296</v>
+            <v>148</v>
           </cell>
           <cell r="L14">
-            <v>400</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="15">
           <cell r="B15" t="str">
-            <v>小冠太阳鱼</v>
+            <v>绿太阳鱼</v>
           </cell>
           <cell r="C15" t="str">
             <v>保底</v>
           </cell>
           <cell r="D15">
-            <v>2</v>
+            <v>1</v>
           </cell>
           <cell r="E15">
-            <v>2.2999999999999998</v>
-          </cell>
+            <v>1.7</v>
+          </cell>
+          <cell r="F15"/>
           <cell r="G15">
-            <v>460</v>
+            <v>340</v>
           </cell>
           <cell r="H15" t="str">
             <v>1、2</v>
@@ -1522,30 +1536,31 @@
             <v>2</v>
           </cell>
           <cell r="J15">
-            <v>1000</v>
+            <v>1200</v>
           </cell>
           <cell r="K15">
+            <v>251</v>
+          </cell>
+          <cell r="L15">
             <v>340</v>
-          </cell>
-          <cell r="L15">
-            <v>460</v>
           </cell>
         </row>
         <row r="16">
           <cell r="B16" t="str">
-            <v>美洲西鲱</v>
+            <v>驼背太阳鱼</v>
           </cell>
           <cell r="C16" t="str">
             <v>保底</v>
           </cell>
           <cell r="D16">
-            <v>2</v>
+            <v>1</v>
           </cell>
           <cell r="E16">
-            <v>2</v>
-          </cell>
+            <v>1.5</v>
+          </cell>
+          <cell r="F16"/>
           <cell r="G16">
-            <v>400</v>
+            <v>300</v>
           </cell>
           <cell r="H16" t="str">
             <v>1、2</v>
@@ -1557,15 +1572,15 @@
             <v>1000</v>
           </cell>
           <cell r="K16">
-            <v>296</v>
+            <v>222</v>
           </cell>
           <cell r="L16">
-            <v>400</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="17">
           <cell r="B17" t="str">
-            <v>岩钝鲈</v>
+            <v>蓝鳃太阳鱼</v>
           </cell>
           <cell r="C17" t="str">
             <v>保底</v>
@@ -1576,6 +1591,7 @@
           <cell r="E17">
             <v>2</v>
           </cell>
+          <cell r="F17"/>
           <cell r="G17">
             <v>400</v>
           </cell>
@@ -1586,7 +1602,7 @@
             <v>2</v>
           </cell>
           <cell r="J17">
-            <v>1000</v>
+            <v>1500</v>
           </cell>
           <cell r="K17">
             <v>296</v>
@@ -1597,19 +1613,20 @@
         </row>
         <row r="18">
           <cell r="B18" t="str">
-            <v>弓鳍鱼</v>
+            <v>小冠太阳鱼</v>
           </cell>
           <cell r="C18" t="str">
-            <v>目标</v>
+            <v>保底</v>
           </cell>
           <cell r="D18">
             <v>2</v>
           </cell>
           <cell r="E18">
-            <v>2.5</v>
-          </cell>
+            <v>2.2999999999999998</v>
+          </cell>
+          <cell r="F18"/>
           <cell r="G18">
-            <v>500</v>
+            <v>460</v>
           </cell>
           <cell r="H18" t="str">
             <v>1、2</v>
@@ -1618,33 +1635,34 @@
             <v>2</v>
           </cell>
           <cell r="J18">
-            <v>1000</v>
+            <v>1500</v>
           </cell>
           <cell r="K18">
-            <v>370</v>
+            <v>340</v>
           </cell>
           <cell r="L18">
-            <v>500</v>
+            <v>460</v>
           </cell>
         </row>
         <row r="19">
           <cell r="B19" t="str">
-            <v>黄鲈</v>
+            <v>美洲西鲱</v>
           </cell>
           <cell r="C19" t="str">
-            <v>目标</v>
+            <v>保底</v>
           </cell>
           <cell r="D19">
-            <v>3</v>
+            <v>2</v>
           </cell>
           <cell r="E19">
-            <v>3.3</v>
-          </cell>
+            <v>2</v>
+          </cell>
+          <cell r="F19"/>
           <cell r="G19">
-            <v>900</v>
+            <v>400</v>
           </cell>
           <cell r="H19" t="str">
-            <v>1、2、3</v>
+            <v>1、2</v>
           </cell>
           <cell r="I19">
             <v>2</v>
@@ -1653,30 +1671,31 @@
             <v>1000</v>
           </cell>
           <cell r="K19">
-            <v>666</v>
+            <v>296</v>
           </cell>
           <cell r="L19">
-            <v>900</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="20">
           <cell r="B20" t="str">
-            <v>红鳍狗鱼</v>
+            <v>岩钝鲈</v>
           </cell>
           <cell r="C20" t="str">
-            <v>目标</v>
+            <v>保底</v>
           </cell>
           <cell r="D20">
-            <v>3</v>
+            <v>2</v>
           </cell>
           <cell r="E20">
-            <v>3.5</v>
-          </cell>
+            <v>2</v>
+          </cell>
+          <cell r="F20"/>
           <cell r="G20">
-            <v>1000</v>
+            <v>400</v>
           </cell>
           <cell r="H20" t="str">
-            <v>1、2、3</v>
+            <v>1、2</v>
           </cell>
           <cell r="I20">
             <v>2</v>
@@ -1685,30 +1704,31 @@
             <v>1000</v>
           </cell>
           <cell r="K20">
-            <v>740</v>
+            <v>296</v>
           </cell>
           <cell r="L20">
-            <v>1000</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="21">
           <cell r="B21" t="str">
-            <v>斑点黑鲈</v>
+            <v>弓鳍鱼</v>
           </cell>
           <cell r="C21" t="str">
             <v>目标</v>
           </cell>
           <cell r="D21">
-            <v>4</v>
+            <v>2</v>
           </cell>
           <cell r="E21">
-            <v>4.5</v>
-          </cell>
+            <v>2.5</v>
+          </cell>
+          <cell r="F21"/>
           <cell r="G21">
-            <v>2000</v>
+            <v>500</v>
           </cell>
           <cell r="H21" t="str">
-            <v>1、2、3、4</v>
+            <v>1、2</v>
           </cell>
           <cell r="I21">
             <v>2</v>
@@ -1717,30 +1737,31 @@
             <v>1000</v>
           </cell>
           <cell r="K21">
-            <v>1480</v>
+            <v>370</v>
           </cell>
           <cell r="L21">
-            <v>2000</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="22">
           <cell r="B22" t="str">
-            <v>大口黑鲈</v>
+            <v>黄鲈</v>
           </cell>
           <cell r="C22" t="str">
             <v>目标</v>
           </cell>
           <cell r="D22">
-            <v>5</v>
+            <v>3</v>
           </cell>
           <cell r="E22">
-            <v>5</v>
-          </cell>
+            <v>3.3</v>
+          </cell>
+          <cell r="F22"/>
           <cell r="G22">
-            <v>3200</v>
+            <v>900</v>
           </cell>
           <cell r="H22" t="str">
-            <v>1、2、3、4、5</v>
+            <v>1、2、3</v>
           </cell>
           <cell r="I22">
             <v>2</v>
@@ -1749,33 +1770,31 @@
             <v>1000</v>
           </cell>
           <cell r="K22">
-            <v>2368</v>
+            <v>666</v>
           </cell>
           <cell r="L22">
-            <v>3200</v>
+            <v>900</v>
           </cell>
         </row>
         <row r="23">
           <cell r="B23" t="str">
-            <v>美洲鳗鲡</v>
+            <v>红鳍狗鱼</v>
           </cell>
           <cell r="C23" t="str">
             <v>目标</v>
           </cell>
           <cell r="D23">
-            <v>5</v>
+            <v>3</v>
           </cell>
           <cell r="E23">
-            <v>5</v>
-          </cell>
-          <cell r="F23" t="str">
-            <v>2场的浮钓，深坑底钓</v>
-          </cell>
+            <v>3.5</v>
+          </cell>
+          <cell r="F23"/>
           <cell r="G23">
-            <v>3200</v>
+            <v>1000</v>
           </cell>
           <cell r="H23" t="str">
-            <v>1、2、3、4、5</v>
+            <v>1、2、3</v>
           </cell>
           <cell r="I23">
             <v>2</v>
@@ -1784,30 +1803,31 @@
             <v>1000</v>
           </cell>
           <cell r="K23">
-            <v>2368</v>
+            <v>740</v>
           </cell>
           <cell r="L23">
-            <v>3200</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="24">
           <cell r="B24" t="str">
-            <v>玻璃梭鲈</v>
+            <v>斑点黑鲈</v>
           </cell>
           <cell r="C24" t="str">
             <v>目标</v>
           </cell>
           <cell r="D24">
-            <v>5</v>
+            <v>4</v>
           </cell>
           <cell r="E24">
-            <v>5.3</v>
-          </cell>
+            <v>4.5</v>
+          </cell>
+          <cell r="F24"/>
           <cell r="G24">
-            <v>3800</v>
+            <v>2000</v>
           </cell>
           <cell r="H24" t="str">
-            <v>1、2、3、4、5</v>
+            <v>1、2、3、4</v>
           </cell>
           <cell r="I24">
             <v>2</v>
@@ -1816,9 +1836,110 @@
             <v>1000</v>
           </cell>
           <cell r="K24">
+            <v>1480</v>
+          </cell>
+          <cell r="L24">
+            <v>2000</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>大口黑鲈</v>
+          </cell>
+          <cell r="C25" t="str">
+            <v>目标</v>
+          </cell>
+          <cell r="D25">
+            <v>5</v>
+          </cell>
+          <cell r="E25">
+            <v>5</v>
+          </cell>
+          <cell r="F25"/>
+          <cell r="G25">
+            <v>3200</v>
+          </cell>
+          <cell r="H25" t="str">
+            <v>1、2、3、4、5</v>
+          </cell>
+          <cell r="I25">
+            <v>2</v>
+          </cell>
+          <cell r="J25">
+            <v>1000</v>
+          </cell>
+          <cell r="K25">
+            <v>2368</v>
+          </cell>
+          <cell r="L25">
+            <v>3200</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>美洲鳗鲡</v>
+          </cell>
+          <cell r="C26" t="str">
+            <v>目标</v>
+          </cell>
+          <cell r="D26">
+            <v>5</v>
+          </cell>
+          <cell r="E26">
+            <v>5</v>
+          </cell>
+          <cell r="F26" t="str">
+            <v>2场的浮钓，深坑底钓</v>
+          </cell>
+          <cell r="G26">
+            <v>3200</v>
+          </cell>
+          <cell r="H26" t="str">
+            <v>1、2、3、4、5</v>
+          </cell>
+          <cell r="I26">
+            <v>2</v>
+          </cell>
+          <cell r="J26">
+            <v>1000</v>
+          </cell>
+          <cell r="K26">
+            <v>2368</v>
+          </cell>
+          <cell r="L26">
+            <v>3200</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>玻璃梭鲈</v>
+          </cell>
+          <cell r="C27" t="str">
+            <v>目标</v>
+          </cell>
+          <cell r="D27">
+            <v>5</v>
+          </cell>
+          <cell r="E27">
+            <v>5.3</v>
+          </cell>
+          <cell r="F27"/>
+          <cell r="G27">
+            <v>3800</v>
+          </cell>
+          <cell r="H27" t="str">
+            <v>1、2、3、4、5</v>
+          </cell>
+          <cell r="I27">
+            <v>2</v>
+          </cell>
+          <cell r="J27">
+            <v>1000</v>
+          </cell>
+          <cell r="K27">
             <v>2812</v>
           </cell>
-          <cell r="L24">
+          <cell r="L27">
             <v>3800</v>
           </cell>
         </row>
@@ -2148,7 +2269,7 @@
   <dimension ref="A1:X200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75"/>
@@ -7116,9 +7237,9 @@
         <f>VLOOKUP(C64,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="B64" s="11">
+      <c r="B64" s="11" t="e">
         <f>VLOOKUP(C64,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3200</v>
+        <v>#N/A</v>
       </c>
       <c r="C64" s="2" t="str">
         <f>VLOOKUP(D64,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -7196,9 +7317,9 @@
         <f>VLOOKUP(C65,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="B65" s="11">
+      <c r="B65" s="11" t="e">
         <f>VLOOKUP(C65,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3200</v>
+        <v>#N/A</v>
       </c>
       <c r="C65" s="2" t="str">
         <f>VLOOKUP(D65,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -7276,9 +7397,9 @@
         <f>VLOOKUP(C66,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="B66" s="11">
+      <c r="B66" s="11" t="e">
         <f>VLOOKUP(C66,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3200</v>
+        <v>#N/A</v>
       </c>
       <c r="C66" s="2" t="str">
         <f>VLOOKUP(D66,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -7356,9 +7477,9 @@
         <f>VLOOKUP(C67,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="B67" s="11">
+      <c r="B67" s="11" t="e">
         <f>VLOOKUP(C67,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3200</v>
+        <v>#N/A</v>
       </c>
       <c r="C67" s="2" t="str">
         <f>VLOOKUP(D67,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -7436,9 +7557,9 @@
         <f>VLOOKUP(C68,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="B68" s="11">
+      <c r="B68" s="11" t="e">
         <f>VLOOKUP(C68,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3200</v>
+        <v>#N/A</v>
       </c>
       <c r="C68" s="2" t="str">
         <f>VLOOKUP(D68,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -7516,9 +7637,9 @@
         <f>VLOOKUP(C69,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="B69" s="11">
+      <c r="B69" s="11" t="e">
         <f>VLOOKUP(C69,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3200</v>
+        <v>#N/A</v>
       </c>
       <c r="C69" s="2" t="str">
         <f>VLOOKUP(D69,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -7596,9 +7717,9 @@
         <f>VLOOKUP(C70,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="B70" s="11">
+      <c r="B70" s="11" t="e">
         <f>VLOOKUP(C70,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3200</v>
+        <v>#N/A</v>
       </c>
       <c r="C70" s="2" t="str">
         <f>VLOOKUP(D70,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -7676,9 +7797,9 @@
         <f>VLOOKUP(C71,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="B71" s="11">
+      <c r="B71" s="11" t="e">
         <f>VLOOKUP(C71,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3200</v>
+        <v>#N/A</v>
       </c>
       <c r="C71" s="2" t="str">
         <f>VLOOKUP(D71,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -7756,9 +7877,9 @@
         <f>VLOOKUP(C72,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="B72" s="11">
+      <c r="B72" s="11" t="e">
         <f>VLOOKUP(C72,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3200</v>
+        <v>#N/A</v>
       </c>
       <c r="C72" s="2" t="str">
         <f>VLOOKUP(D72,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -7836,9 +7957,9 @@
         <f>VLOOKUP(C73,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="B73" s="11">
+      <c r="B73" s="11" t="e">
         <f>VLOOKUP(C73,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3200</v>
+        <v>#N/A</v>
       </c>
       <c r="C73" s="2" t="str">
         <f>VLOOKUP(D73,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -7916,9 +8037,9 @@
         <f>VLOOKUP(C74,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5.3</v>
       </c>
-      <c r="B74" s="11">
+      <c r="B74" s="11" t="e">
         <f>VLOOKUP(C74,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3800</v>
+        <v>#N/A</v>
       </c>
       <c r="C74" s="2" t="str">
         <f>VLOOKUP(D74,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -7996,9 +8117,9 @@
         <f>VLOOKUP(C75,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5.3</v>
       </c>
-      <c r="B75" s="11">
+      <c r="B75" s="11" t="e">
         <f>VLOOKUP(C75,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3800</v>
+        <v>#N/A</v>
       </c>
       <c r="C75" s="2" t="str">
         <f>VLOOKUP(D75,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -8076,9 +8197,9 @@
         <f>VLOOKUP(C76,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5.3</v>
       </c>
-      <c r="B76" s="11">
+      <c r="B76" s="11" t="e">
         <f>VLOOKUP(C76,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3800</v>
+        <v>#N/A</v>
       </c>
       <c r="C76" s="2" t="str">
         <f>VLOOKUP(D76,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -8156,9 +8277,9 @@
         <f>VLOOKUP(C77,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5.3</v>
       </c>
-      <c r="B77" s="11">
+      <c r="B77" s="11" t="e">
         <f>VLOOKUP(C77,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3800</v>
+        <v>#N/A</v>
       </c>
       <c r="C77" s="2" t="str">
         <f>VLOOKUP(D77,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>
@@ -8236,9 +8357,9 @@
         <f>VLOOKUP(C78,[1]鱼种设计表!$B$2:$L$55,4,FALSE)</f>
         <v>5.3</v>
       </c>
-      <c r="B78" s="11">
+      <c r="B78" s="11" t="e">
         <f>VLOOKUP(C78,[1]鱼种设计表!$B$2:$L$24,11,FALSE)</f>
-        <v>3800</v>
+        <v>#N/A</v>
       </c>
       <c r="C78" s="2" t="str">
         <f>VLOOKUP(D78,鱼种重量参数!$A$1:$D$99,4,FALSE)</f>

</xml_diff>